<commit_message>
learning java silver section 2
</commit_message>
<xml_diff>
--- a/Java/java se silver/演習、模試記録.xlsx
+++ b/Java/java se silver/演習、模試記録.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\tomohiro-odan\git\Competitive-programming\Java\java se silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4BBB1-FA5F-4AD0-BCB1-5371B661F41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E115CFF2-FEE2-4B5C-AD36-C995F0029E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="327">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -1242,6 +1242,45 @@
   </si>
   <si>
     <t>2-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A,B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キャストとかの時を思い出して</t>
+    <rPh sb="7" eb="8">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>valueOfは特殊</t>
+    <rPh sb="8" eb="10">
+      <t>トクシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>予想外</t>
+    <rPh sb="0" eb="3">
+      <t>ヨソウガイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>capacityとはなにか…</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1769,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA50DF-B315-4988-A79E-78C13B408B2B}">
   <dimension ref="A1:L183"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1795,7 +1834,7 @@
       </c>
       <c r="E1" s="13">
         <f t="shared" ref="E1:F1" si="0">COUNTIF(E4:E402,"〇")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="13">
         <f t="shared" si="0"/>
@@ -1815,7 +1854,7 @@
       </c>
       <c r="E2" s="29">
         <f>1-E1/(COUNTA($B:$B)-1)</f>
-        <v>0.97222222222222221</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="F2" s="29">
         <f>1-F1/(COUNTA($B:$B)-1)</f>
@@ -2117,27 +2156,37 @@
         <v>82</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F19" s="15"/>
-      <c r="G19" s="26"/>
+      <c r="G19" s="26" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="32"/>
       <c r="B20" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="26"/>
+      <c r="G20" s="26" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="32"/>
       <c r="B21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D21" s="15" t="s">
         <v>3</v>
       </c>
@@ -2150,9 +2199,13 @@
       <c r="B22" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F22" s="15"/>
       <c r="G22" s="26"/>
     </row>
@@ -2161,7 +2214,9 @@
       <c r="B23" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -2172,7 +2227,9 @@
       <c r="B24" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -2183,7 +2240,9 @@
       <c r="B25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -2194,9 +2253,13 @@
       <c r="B26" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="E26" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F26" s="15"/>
       <c r="G26" s="26"/>
     </row>
@@ -2205,7 +2268,9 @@
       <c r="B27" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -2216,7 +2281,9 @@
       <c r="B28" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -2227,7 +2294,9 @@
       <c r="B29" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -2238,33 +2307,43 @@
       <c r="B30" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D30" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="26"/>
+      <c r="G30" s="26" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="32"/>
       <c r="B31" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="26" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="32"/>
       <c r="B32" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
@@ -2275,7 +2354,9 @@
       <c r="B33" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -4125,17 +4206,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A33"/>
-    <mergeCell ref="A34:A54"/>
-    <mergeCell ref="A55:A71"/>
-    <mergeCell ref="A72:A81"/>
     <mergeCell ref="A82:A111"/>
     <mergeCell ref="A160:A176"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A133:A140"/>
     <mergeCell ref="A141:A159"/>
     <mergeCell ref="A112:A132"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A33"/>
+    <mergeCell ref="A34:A54"/>
+    <mergeCell ref="A55:A71"/>
+    <mergeCell ref="A72:A81"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
learning java silver section 8
</commit_message>
<xml_diff>
--- a/Java/java se silver/演習、模試記録.xlsx
+++ b/Java/java se silver/演習、模試記録.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\tomohiro-odan\git\Competitive-programming\Java\java se silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E115CFF2-FEE2-4B5C-AD36-C995F0029E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2EAEF9-7419-4882-8792-6713D6357E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="372" yWindow="2604" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="問題集の苦手分野" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="332">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -1281,6 +1281,38 @@
   </si>
   <si>
     <t>capacityとはなにか…</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2つ選択なのを忘れずに</t>
+    <rPh sb="2" eb="4">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ワス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>誤っているものを選ぶ</t>
+    <rPh sb="0" eb="1">
+      <t>アヤマ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BC</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1808,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA50DF-B315-4988-A79E-78C13B408B2B}">
   <dimension ref="A1:L183"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1834,7 +1866,7 @@
       </c>
       <c r="E1" s="13">
         <f t="shared" ref="E1:F1" si="0">COUNTIF(E4:E402,"〇")</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F1" s="13">
         <f t="shared" si="0"/>
@@ -1854,7 +1886,7 @@
       </c>
       <c r="E2" s="29">
         <f>1-E1/(COUNTA($B:$B)-1)</f>
-        <v>0.9555555555555556</v>
+        <v>0.92222222222222228</v>
       </c>
       <c r="F2" s="29">
         <f>1-F1/(COUNTA($B:$B)-1)</f>
@@ -3579,7 +3611,9 @@
       <c r="B133" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C133" s="17"/>
+      <c r="C133" s="17" t="s">
+        <v>329</v>
+      </c>
       <c r="D133" s="15" t="s">
         <v>3</v>
       </c>
@@ -3592,20 +3626,26 @@
       <c r="B134" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C134" s="17"/>
+      <c r="C134" s="17" t="s">
+        <v>331</v>
+      </c>
       <c r="D134" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E134" s="15"/>
       <c r="F134" s="15"/>
-      <c r="G134" s="26"/>
+      <c r="G134" s="26" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="32"/>
       <c r="B135" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C135" s="17"/>
+      <c r="C135" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D135" s="15" t="s">
         <v>3</v>
       </c>
@@ -3618,7 +3658,9 @@
       <c r="B136" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C136" s="17"/>
+      <c r="C136" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
       <c r="F136" s="15"/>
@@ -3629,11 +3671,15 @@
       <c r="B137" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C137" s="17"/>
+      <c r="C137" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D137" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E137" s="15"/>
+      <c r="E137" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F137" s="15"/>
       <c r="G137" s="26"/>
       <c r="I137" s="18"/>
@@ -3643,11 +3689,15 @@
       <c r="B138" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C138" s="17"/>
+      <c r="C138" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D138" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E138" s="15"/>
+      <c r="E138" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F138" s="15"/>
       <c r="G138" s="26"/>
     </row>
@@ -3656,7 +3706,9 @@
       <c r="B139" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C139" s="17"/>
+      <c r="C139" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
       <c r="F139" s="15"/>
@@ -3668,11 +3720,15 @@
       <c r="B140" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="C140" s="17"/>
+      <c r="C140" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D140" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E140" s="15"/>
+      <c r="E140" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F140" s="15"/>
       <c r="G140" s="26"/>
       <c r="I140" s="21"/>
@@ -4124,7 +4180,9 @@
       <c r="B177" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C177" s="17"/>
+      <c r="C177" s="17" t="s">
+        <v>327</v>
+      </c>
       <c r="D177" s="15" t="s">
         <v>3</v>
       </c>
@@ -4137,11 +4195,15 @@
       <c r="B178" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C178" s="17"/>
+      <c r="C178" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D178" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E178" s="15"/>
+      <c r="E178" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F178" s="15"/>
       <c r="G178" s="26"/>
     </row>
@@ -4150,7 +4212,9 @@
       <c r="B179" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C179" s="17"/>
+      <c r="C179" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
       <c r="F179" s="15"/>
@@ -4161,11 +4225,15 @@
       <c r="B180" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C180" s="17"/>
+      <c r="C180" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D180" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E180" s="15"/>
+      <c r="E180" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F180" s="15"/>
       <c r="G180" s="26"/>
     </row>
@@ -4174,9 +4242,13 @@
       <c r="B181" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="C181" s="17"/>
+      <c r="C181" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D181" s="15"/>
-      <c r="E181" s="15"/>
+      <c r="E181" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F181" s="15"/>
       <c r="G181" s="26"/>
     </row>
@@ -4185,20 +4257,26 @@
       <c r="B182" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="C182" s="17"/>
+      <c r="C182" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D182" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E182" s="15"/>
       <c r="F182" s="15"/>
-      <c r="G182" s="26"/>
+      <c r="G182" s="26" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" s="33"/>
       <c r="B183" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C183" s="17"/>
+      <c r="C183" s="17" t="s">
+        <v>322</v>
+      </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
       <c r="F183" s="15"/>
@@ -4206,17 +4284,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A33"/>
+    <mergeCell ref="A34:A54"/>
+    <mergeCell ref="A55:A71"/>
+    <mergeCell ref="A72:A81"/>
     <mergeCell ref="A82:A111"/>
     <mergeCell ref="A160:A176"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A133:A140"/>
     <mergeCell ref="A141:A159"/>
     <mergeCell ref="A112:A132"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A33"/>
-    <mergeCell ref="A34:A54"/>
-    <mergeCell ref="A55:A71"/>
-    <mergeCell ref="A72:A81"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
learning java silver chapter 3
</commit_message>
<xml_diff>
--- a/Java/java se silver/演習、模試記録.xlsx
+++ b/Java/java se silver/演習、模試記録.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\tomohiro-odan\git\Competitive-programming\Java\java se silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2EAEF9-7419-4882-8792-6713D6357E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A2EB1-7089-4AB2-875E-D009F03C449E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="2604" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="問題集の苦手分野" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="334">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -1241,10 +1241,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2-8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>A,B</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1313,6 +1309,21 @@
   </si>
   <si>
     <t>BC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CAD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FH以外</t>
+    <rPh sb="2" eb="4">
+      <t>イガイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>３</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1841,7 +1852,7 @@
   <dimension ref="A1:L183"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1866,7 +1877,7 @@
       </c>
       <c r="E1" s="13">
         <f t="shared" ref="E1:F1" si="0">COUNTIF(E4:E402,"〇")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="13">
         <f t="shared" si="0"/>
@@ -1886,7 +1897,7 @@
       </c>
       <c r="E2" s="29">
         <f>1-E1/(COUNTA($B:$B)-1)</f>
-        <v>0.92222222222222228</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F2" s="29">
         <f>1-F1/(COUNTA($B:$B)-1)</f>
@@ -1923,7 +1934,7 @@
         <v>62</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>64</v>
@@ -2193,7 +2204,7 @@
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2202,13 +2213,13 @@
         <v>90</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2217,7 +2228,7 @@
         <v>91</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>3</v>
@@ -2301,7 +2312,7 @@
         <v>95</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -2314,7 +2325,7 @@
         <v>96</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
@@ -2348,7 +2359,7 @@
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2365,7 +2376,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2387,7 +2398,7 @@
         <v>101</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
@@ -2401,7 +2412,9 @@
       <c r="B34" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2412,7 +2425,9 @@
       <c r="B35" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D35" s="15" t="s">
         <v>3</v>
       </c>
@@ -2425,7 +2440,9 @@
       <c r="B36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="17" t="s">
+        <v>331</v>
+      </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
@@ -2436,7 +2453,9 @@
       <c r="B37" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2447,7 +2466,9 @@
       <c r="B38" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
@@ -2458,7 +2479,9 @@
       <c r="B39" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D39" s="15" t="s">
         <v>3</v>
       </c>
@@ -2471,7 +2494,9 @@
       <c r="B40" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
@@ -2482,7 +2507,9 @@
       <c r="B41" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -2493,7 +2520,9 @@
       <c r="B42" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D42" s="15" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2535,9 @@
       <c r="B43" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D43" s="15" t="s">
         <v>3</v>
       </c>
@@ -2519,7 +2550,9 @@
       <c r="B44" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D44" s="15" t="s">
         <v>3</v>
       </c>
@@ -2532,7 +2565,9 @@
       <c r="B45" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
@@ -2543,7 +2578,9 @@
       <c r="B46" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D46" s="15" t="s">
         <v>178</v>
       </c>
@@ -2558,7 +2595,9 @@
       <c r="B47" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D47" s="15" t="s">
         <v>3</v>
       </c>
@@ -2571,7 +2610,9 @@
       <c r="B48" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
@@ -2582,7 +2623,9 @@
       <c r="B49" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D49" s="15" t="s">
         <v>3</v>
       </c>
@@ -2595,7 +2638,9 @@
       <c r="B50" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
@@ -2606,7 +2651,9 @@
       <c r="B51" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="17"/>
+      <c r="C51" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -2617,11 +2664,15 @@
       <c r="B52" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="17"/>
+      <c r="C52" s="17" t="s">
+        <v>332</v>
+      </c>
       <c r="D52" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="15"/>
+      <c r="E52" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F52" s="15"/>
       <c r="G52" s="26"/>
     </row>
@@ -2630,7 +2681,9 @@
       <c r="B53" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="17"/>
+      <c r="C53" s="17" t="s">
+        <v>326</v>
+      </c>
       <c r="D53" s="15" t="s">
         <v>3</v>
       </c>
@@ -2643,7 +2696,9 @@
       <c r="B54" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="17"/>
+      <c r="C54" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D54" s="15" t="s">
         <v>3</v>
       </c>
@@ -3612,7 +3667,7 @@
         <v>135</v>
       </c>
       <c r="C133" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>3</v>
@@ -3627,7 +3682,7 @@
         <v>143</v>
       </c>
       <c r="C134" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>3</v>
@@ -3635,7 +3690,7 @@
       <c r="E134" s="15"/>
       <c r="F134" s="15"/>
       <c r="G134" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4181,7 +4236,7 @@
         <v>138</v>
       </c>
       <c r="C177" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>3</v>
@@ -4243,7 +4298,7 @@
         <v>175</v>
       </c>
       <c r="C181" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
@@ -4266,7 +4321,7 @@
       <c r="E182" s="15"/>
       <c r="F182" s="15"/>
       <c r="G182" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4275,7 +4330,7 @@
         <v>177</v>
       </c>
       <c r="C183" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>

</xml_diff>

<commit_message>
learning silver chapter 5
</commit_message>
<xml_diff>
--- a/Java/java se silver/演習、模試記録.xlsx
+++ b/Java/java se silver/演習、模試記録.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\tomohiro-odan\git\Competitive-programming\Java\java se silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A2EB1-7089-4AB2-875E-D009F03C449E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFAAC68-B25D-46A6-BBFA-9586B9C53749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="338">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -1324,6 +1324,22 @@
   </si>
   <si>
     <t>３</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BEF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AD</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1851,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA50DF-B315-4988-A79E-78C13B408B2B}">
   <dimension ref="A1:L183"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1877,7 +1893,7 @@
       </c>
       <c r="E1" s="13">
         <f t="shared" ref="E1:F1" si="0">COUNTIF(E4:E402,"〇")</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F1" s="13">
         <f t="shared" si="0"/>
@@ -1897,7 +1913,7 @@
       </c>
       <c r="E2" s="29">
         <f>1-E1/(COUNTA($B:$B)-1)</f>
-        <v>0.91666666666666663</v>
+        <v>0.9</v>
       </c>
       <c r="F2" s="29">
         <f>1-F1/(COUNTA($B:$B)-1)</f>
@@ -2917,7 +2933,9 @@
       <c r="B72" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C72" s="17"/>
+      <c r="C72" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D72" s="15" t="s">
         <v>3</v>
       </c>
@@ -2930,7 +2948,9 @@
       <c r="B73" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C73" s="17"/>
+      <c r="C73" s="17" t="s">
+        <v>334</v>
+      </c>
       <c r="D73" s="15" t="s">
         <v>3</v>
       </c>
@@ -2943,11 +2963,15 @@
       <c r="B74" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="17"/>
+      <c r="C74" s="17" t="s">
+        <v>335</v>
+      </c>
       <c r="D74" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E74" s="15"/>
+      <c r="E74" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F74" s="15"/>
       <c r="G74" s="26"/>
     </row>
@@ -2956,11 +2980,15 @@
       <c r="B75" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C75" s="17"/>
+      <c r="C75" s="17" t="s">
+        <v>336</v>
+      </c>
       <c r="D75" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F75" s="15"/>
       <c r="G75" s="26"/>
     </row>
@@ -2969,7 +2997,9 @@
       <c r="B76" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C76" s="17"/>
+      <c r="C76" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D76" s="15" t="s">
         <v>3</v>
       </c>
@@ -2982,7 +3012,9 @@
       <c r="B77" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="17"/>
+      <c r="C77" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D77" s="15" t="s">
         <v>3</v>
       </c>
@@ -2995,11 +3027,15 @@
       <c r="B78" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C78" s="17"/>
+      <c r="C78" s="17" t="s">
+        <v>337</v>
+      </c>
       <c r="D78" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F78" s="15"/>
       <c r="G78" s="26"/>
     </row>
@@ -3008,7 +3044,9 @@
       <c r="B79" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C79" s="17"/>
+      <c r="C79" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D79" s="15" t="s">
         <v>3</v>
       </c>
@@ -3021,7 +3059,9 @@
       <c r="B80" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="17"/>
+      <c r="C80" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D80" s="15" t="s">
         <v>3</v>
       </c>
@@ -3034,7 +3074,9 @@
       <c r="B81" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C81" s="17"/>
+      <c r="C81" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
       <c r="F81" s="15"/>
@@ -4339,17 +4381,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A33"/>
-    <mergeCell ref="A34:A54"/>
-    <mergeCell ref="A55:A71"/>
-    <mergeCell ref="A72:A81"/>
     <mergeCell ref="A82:A111"/>
     <mergeCell ref="A160:A176"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A133:A140"/>
     <mergeCell ref="A141:A159"/>
     <mergeCell ref="A112:A132"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A33"/>
+    <mergeCell ref="A34:A54"/>
+    <mergeCell ref="A55:A71"/>
+    <mergeCell ref="A72:A81"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
learning silver chapter 4
</commit_message>
<xml_diff>
--- a/Java/java se silver/演習、模試記録.xlsx
+++ b/Java/java se silver/演習、模試記録.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\tomohiro-odan\git\Competitive-programming\Java\java se silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFAAC68-B25D-46A6-BBFA-9586B9C53749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A4D17C-B0FE-44EA-8E62-2BEEDFB75D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="340">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -1323,10 +1323,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>３</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>G</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1340,6 +1336,18 @@
   </si>
   <si>
     <t>AD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ACD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ラベルとは…</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1867,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CA50DF-B315-4988-A79E-78C13B408B2B}">
   <dimension ref="A1:L183"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1893,7 +1901,7 @@
       </c>
       <c r="E1" s="13">
         <f t="shared" ref="E1:F1" si="0">COUNTIF(E4:E402,"〇")</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F1" s="13">
         <f t="shared" si="0"/>
@@ -1913,7 +1921,7 @@
       </c>
       <c r="E2" s="29">
         <f>1-E1/(COUNTA($B:$B)-1)</f>
-        <v>0.9</v>
+        <v>0.87777777777777777</v>
       </c>
       <c r="F2" s="29">
         <f>1-F1/(COUNTA($B:$B)-1)</f>
@@ -1950,7 +1958,7 @@
         <v>62</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>64</v>
@@ -2729,7 +2737,9 @@
       <c r="B55" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="17"/>
+      <c r="C55" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
@@ -2740,7 +2750,9 @@
       <c r="B56" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C56" s="17"/>
+      <c r="C56" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
@@ -2751,9 +2763,13 @@
       <c r="B57" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="17"/>
+      <c r="C57" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="E57" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F57" s="15"/>
       <c r="G57" s="26"/>
     </row>
@@ -2762,7 +2778,9 @@
       <c r="B58" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="17"/>
+      <c r="C58" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
@@ -2773,7 +2791,9 @@
       <c r="B59" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="17"/>
+      <c r="C59" s="17" t="s">
+        <v>317</v>
+      </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
@@ -2784,7 +2804,9 @@
       <c r="B60" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="17"/>
+      <c r="C60" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
@@ -2795,11 +2817,15 @@
       <c r="B61" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="17"/>
+      <c r="C61" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D61" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="15"/>
+      <c r="E61" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F61" s="15"/>
       <c r="G61" s="26"/>
       <c r="I61" s="18"/>
@@ -2809,7 +2835,9 @@
       <c r="B62" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C62" s="17"/>
+      <c r="C62" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D62" s="15" t="s">
         <v>3</v>
       </c>
@@ -2822,7 +2850,9 @@
       <c r="B63" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="17"/>
+      <c r="C63" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="D63" s="15" t="s">
         <v>3</v>
       </c>
@@ -2835,7 +2865,9 @@
       <c r="B64" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="17"/>
+      <c r="C64" s="17" t="s">
+        <v>337</v>
+      </c>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
@@ -2846,9 +2878,13 @@
       <c r="B65" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="17"/>
+      <c r="C65" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
+      <c r="E65" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F65" s="15"/>
       <c r="G65" s="26"/>
     </row>
@@ -2857,7 +2893,9 @@
       <c r="B66" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="17"/>
+      <c r="C66" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
@@ -2868,11 +2906,15 @@
       <c r="B67" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="17"/>
+      <c r="C67" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D67" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="15"/>
+      <c r="E67" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="F67" s="15"/>
       <c r="G67" s="26"/>
     </row>
@@ -2881,7 +2923,9 @@
       <c r="B68" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="17"/>
+      <c r="C68" s="17" t="s">
+        <v>321</v>
+      </c>
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="15"/>
@@ -2892,7 +2936,9 @@
       <c r="B69" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="17"/>
+      <c r="C69" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D69" s="15" t="s">
         <v>3</v>
       </c>
@@ -2905,20 +2951,26 @@
       <c r="B70" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C70" s="17"/>
+      <c r="C70" s="17" t="s">
+        <v>334</v>
+      </c>
       <c r="D70" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E70" s="15"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="26"/>
+      <c r="G70" s="26" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="33"/>
       <c r="B71" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="17"/>
+      <c r="C71" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D71" s="15" t="s">
         <v>3</v>
       </c>
@@ -2949,7 +3001,7 @@
         <v>140</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>3</v>
@@ -2964,7 +3016,7 @@
         <v>40</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>3</v>
@@ -2981,7 +3033,7 @@
         <v>41</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>3</v>
@@ -3028,7 +3080,7 @@
         <v>43</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>3</v>

</xml_diff>